<commit_message>
Test specifications document added
</commit_message>
<xml_diff>
--- a/gilden_rose.xlsx
+++ b/gilden_rose.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://logirail-my.sharepoint.com/personal/anton_stamov_logirail_com/Documents/Projects/Formacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="570" documentId="8_{76D17780-8A6E-47AF-812E-C6A780C72E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{119574A4-BF21-4390-A582-B33D4639E6FB}"/>
+  <xr:revisionPtr revIDLastSave="572" documentId="8_{76D17780-8A6E-47AF-812E-C6A780C72E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00C70BBA-A3A4-4F8E-A0EE-241728FE82FF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{92436C35-48CE-4FCA-887F-D58C2DF8B26B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{92436C35-48CE-4FCA-887F-D58C2DF8B26B}"/>
   </bookViews>
   <sheets>
     <sheet name="item" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="58">
   <si>
     <t>C1</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Aged brie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -444,9 +447,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -471,9 +473,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -498,14 +497,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -532,7 +527,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -552,6 +547,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,55 +593,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,262 +911,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59EAAD5-3698-40E6-A027-CB4EA784CD80}">
-  <dimension ref="B2:K22"/>
+  <dimension ref="B2:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="11"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="13" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B2" s="10"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="36" t="s">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="42" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="67" t="s">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="69"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="34"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="42" t="s">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="56"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="28"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="42" t="s">
+      <c r="D7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="16"/>
-      <c r="K8" s="17"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="42" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="42" t="s">
+      <c r="D9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="67"/>
-      <c r="C11" s="37" t="s">
+      <c r="D10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="54"/>
+      <c r="C11" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" s="19"/>
-    </row>
-    <row r="13" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="16"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="17"/>
+      <c r="N11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -1193,250 +1179,250 @@
       <c r="J13"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="21"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="13" t="s">
+    <row r="14" spans="2:14" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="19"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="51" t="s">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="J15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="52"/>
-      <c r="C16" s="46" t="s">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="43"/>
+      <c r="C16" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16">
         <v>4</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16">
         <v>3</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16">
         <v>2</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16">
         <v>-1</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16">
         <v>-2</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16">
         <v>-3</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="6">
         <v>-1</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="53"/>
-      <c r="C17" s="47" t="s">
+      <c r="B17" s="44"/>
+      <c r="C17" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="1">
         <v>3</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="1">
         <v>-1</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H17" s="1">
         <v>1</v>
       </c>
-      <c r="I17" s="27">
+      <c r="I17" s="1">
         <v>7</v>
       </c>
-      <c r="J17" s="27">
+      <c r="J17" s="1">
         <v>0</v>
       </c>
-      <c r="K17" s="28">
+      <c r="K17" s="7">
         <v>-3</v>
       </c>
     </row>
-    <row r="18" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="70"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="41"/>
+    <row r="18" spans="2:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="57"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="35"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I19" s="23" t="s">
+      <c r="I19" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="23" t="s">
+      <c r="J19" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="24" t="s">
+      <c r="K19" s="22" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="52"/>
-      <c r="C20" s="46" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20">
         <v>3</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="24">
         <v>3</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20">
         <v>1</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20">
         <v>-2</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20">
         <v>-3</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20">
         <f>J16</f>
         <v>-3</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="6">
         <f>K16-1</f>
         <v>-2</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="52"/>
-      <c r="C21" s="46" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="24">
         <v>-1</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21">
         <v>0</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21">
         <v>0</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21">
         <v>5</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21">
         <f>J17</f>
         <v>0</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="53"/>
-      <c r="C22" s="29" t="s">
+      <c r="B22" s="44"/>
+      <c r="C22" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12" t="s">
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12" t="s">
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K22" s="35"/>
+      <c r="K22" s="29"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1447,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574E3CEC-5933-4FC9-939C-608C87537969}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A2:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,316 +1445,303 @@
     <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="21"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="65" t="s">
+    <row r="2" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="19"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="E2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="68"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
-      <c r="K5" s="3"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="10"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="G7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="57" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="67" t="s">
+      <c r="D8" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="29" t="s">
+      <c r="D9" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="31"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="61"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="13" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="25"/>
+    </row>
+    <row r="13" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="48"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="49"/>
-      <c r="C15" s="38" t="s">
+      <c r="B15" s="61"/>
+      <c r="C15" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>3</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
         <v>-1</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <v>-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="50"/>
-      <c r="C16" s="37" t="s">
+      <c r="B16" s="62"/>
+      <c r="C16" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>50</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>49</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>25</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="71"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="72"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="59"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="49"/>
-      <c r="C19" s="38" t="s">
+      <c r="B19" s="61"/>
+      <c r="C19" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>2</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19">
         <v>-2</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>-1</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>-3</v>
       </c>
-      <c r="I19" s="10"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="50"/>
-      <c r="C20" s="37" t="s">
+      <c r="B20" s="62"/>
+      <c r="C20" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>50</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>50</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>26</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>35</v>
       </c>
     </row>

</xml_diff>